<commit_message>
Completed leetcode 114 using better approach and refactored problems with Tree structure for testing.
</commit_message>
<xml_diff>
--- a/RevisionSheet.xlsx
+++ b/RevisionSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milind.gokhale/github/jsdev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F34D390-65FB-B14D-B4CB-E0909C6C16F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5FDB0F-F528-E54F-95F8-EB10B084A783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{20D34E75-82C1-E34C-A7B5-A57F903BD2B5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19360" xr2:uid="{20D34E75-82C1-E34C-A7B5-A57F903BD2B5}"/>
   </bookViews>
   <sheets>
     <sheet name="LC" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="117">
   <si>
     <t>#</t>
   </si>
@@ -191,12 +191,213 @@
   <si>
     <t>Simple linkedlist pointers</t>
   </si>
+  <si>
+    <t>Unique Paths</t>
+  </si>
+  <si>
+    <t>Unique Paths II</t>
+  </si>
+  <si>
+    <t>Same as 63 and 62</t>
+  </si>
+  <si>
+    <t>Minimum Path Sum</t>
+  </si>
+  <si>
+    <t>Plus One</t>
+  </si>
+  <si>
+    <t>Too easy</t>
+  </si>
+  <si>
+    <t>Add Binary</t>
+  </si>
+  <si>
+    <t>Array | Linear | String</t>
+  </si>
+  <si>
+    <t>Very easy. But simplify in single while loop instead of 3 loops. Since its for array and not for a list. That makes the code much more readable.</t>
+  </si>
+  <si>
+    <t>Text Justification</t>
+  </si>
+  <si>
+    <t>Need many revisions of this for a concise and easy to reproduce solution</t>
+  </si>
+  <si>
+    <t>Need more revision. Good problem even though simple</t>
+  </si>
+  <si>
+    <t>Sqrt(x)</t>
+  </si>
+  <si>
+    <t>Climbing Stairs</t>
+  </si>
+  <si>
+    <t>Fibonacci | Numbers | Iterative | Recursion</t>
+  </si>
+  <si>
+    <t>Best way to solve it is iterative way even though the intuition is completely of recursion.</t>
+  </si>
+  <si>
+    <t>Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t>Really good way of reducing space complexity.</t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix</t>
+  </si>
+  <si>
+    <t>I'm liking it. Lovely problem. Consider 2D array as a 1D array instead and do binary search</t>
+  </si>
+  <si>
+    <t>Color Sort | Dutch flag problem</t>
+  </si>
+  <si>
+    <t>Partition Logic | Quicksort | Array | Linear | Pointer play</t>
+  </si>
+  <si>
+    <t>This is really a good problem to understand the basic invariable condition of the quicksort's partition algorithm.</t>
+  </si>
+  <si>
+    <t>Remove duplicates from sorted array II</t>
+  </si>
+  <si>
+    <t>Simple problem with pointers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-number-of-refueling-stops/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/furthest-building-you-can-reach/</t>
+  </si>
+  <si>
+    <t>A very important clue found about problems which are not actually Dynamic Programming - If problem is actually 0/1 Knapsack like problem then it can probably be solved using Greedy Approach than using dynamic programming extra efforts.</t>
+  </si>
+  <si>
+    <t>Remove duplicates from sorted list II</t>
+  </si>
+  <si>
+    <t>LinkedList | Linear | Pointer Play</t>
+  </si>
+  <si>
+    <t>Array | Linear | Index Play</t>
+  </si>
+  <si>
+    <t>Remove duplicates from sorted list</t>
+  </si>
+  <si>
+    <t>Simple problem with pointers/array indices</t>
+  </si>
+  <si>
+    <t>Partition List</t>
+  </si>
+  <si>
+    <t>The crux of the problem is to not needing any array strategy like partition logic used in Dutch flag problem.</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>Array | Array Methods | Linear</t>
+  </si>
+  <si>
+    <t>The main caveat is to do in-place. For this clue is splice method of arrays to inject the smaller element in one of the arrays. Revision MUST!</t>
+  </si>
+  <si>
+    <t>Key is to do it iteratively. Recursion is trivial - LCR</t>
+  </si>
+  <si>
+    <t>Binary Tree inorder traversal</t>
+  </si>
+  <si>
+    <t>Tree | Recursion | Iterative | Pointer Play</t>
+  </si>
+  <si>
+    <t>Same tree</t>
+  </si>
+  <si>
+    <t>Tree | Recursion | Pointer Play</t>
+  </si>
+  <si>
+    <t>Think of base cases of recursion, either of the tree null but not both null and how about both leaf or not leaf nodes</t>
+  </si>
+  <si>
+    <t>Symmetric Tree</t>
+  </si>
+  <si>
+    <t>Recursive is Trivial | But iterative is the key for performance and basically using Level Order Traversal is the trick!!</t>
+  </si>
+  <si>
+    <t>Minimum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>Tree | Recursion | DFS | BFS</t>
+  </si>
+  <si>
+    <t>Trivial to do it using recursion or stack or DFS. But the main trick is to reach first leaf node. So its better to do it in BFS.</t>
+  </si>
+  <si>
+    <t>Flatten Binary Tree to Linked List</t>
+  </si>
+  <si>
+    <t>TRee | Recursion | DFS | BFS | LinkedList</t>
+  </si>
+  <si>
+    <t>Binary Tree Level order traversal</t>
+  </si>
+  <si>
+    <t>Binary Tree zigzag level order traversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tree | BFS | Queue </t>
+  </si>
+  <si>
+    <t>Trivial with queue and sentinel</t>
+  </si>
+  <si>
+    <t>Trivial with 2 stacks and sentinel</t>
+  </si>
+  <si>
+    <t>Tree | BFS | Queue | Stack</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>Tree | DFS | Recursion</t>
+  </si>
+  <si>
+    <t>Binary Tree Level order traversal II</t>
+  </si>
+  <si>
+    <t>Convert sorted array to Binary tree</t>
+  </si>
+  <si>
+    <t>Tree | Recursion | Divide and Conquer</t>
+  </si>
+  <si>
+    <t>DO this by using divie and conquer strategy in recursion.</t>
+  </si>
+  <si>
+    <t>Path Sum</t>
+  </si>
+  <si>
+    <t>Trivial</t>
+  </si>
+  <si>
+    <t>Path Sum II</t>
+  </si>
+  <si>
+    <t>DO it again using the recursive solution using O(1) space. Think of post order to prepare preorder. Inverse iteration pattern</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,6 +409,15 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -240,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -250,6 +460,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -565,13 +776,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E863F9-6DAE-454C-871E-E881AC4B67FC}">
-  <dimension ref="A3:G47"/>
+  <dimension ref="A3:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomRight" activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -902,7 +1113,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -919,7 +1130,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -933,7 +1144,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -944,7 +1155,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -961,7 +1172,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -978,7 +1189,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -995,30 +1206,514 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>63</v>
+      </c>
+      <c r="C40" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>67</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" t="s">
+        <v>57</v>
+      </c>
+      <c r="F43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>68</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>69</v>
+      </c>
+      <c r="C45" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>70</v>
+      </c>
+      <c r="C46" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
       <c r="B47">
+        <v>73</v>
+      </c>
+      <c r="C47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>75</v>
+      </c>
+      <c r="C49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" t="s">
+        <v>71</v>
+      </c>
+      <c r="F49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>80</v>
+      </c>
+      <c r="C50" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" t="s">
+        <v>80</v>
+      </c>
+      <c r="F50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>82</v>
+      </c>
+      <c r="C51" t="s">
+        <v>78</v>
+      </c>
+      <c r="D51" t="s">
+        <v>79</v>
+      </c>
+      <c r="F51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>83</v>
+      </c>
+      <c r="C52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" t="s">
+        <v>79</v>
+      </c>
+      <c r="F52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>86</v>
+      </c>
+      <c r="C53" t="s">
+        <v>83</v>
+      </c>
+      <c r="D53" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>88</v>
+      </c>
+      <c r="C54" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" t="s">
+        <v>86</v>
+      </c>
+      <c r="F54" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>94</v>
+      </c>
+      <c r="C55" t="s">
+        <v>89</v>
+      </c>
+      <c r="D55" t="s">
+        <v>90</v>
+      </c>
+      <c r="F55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>100</v>
+      </c>
+      <c r="C56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" t="s">
+        <v>92</v>
+      </c>
+      <c r="F56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>101</v>
+      </c>
+      <c r="C57" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" t="s">
+        <v>90</v>
+      </c>
+      <c r="F57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>102</v>
+      </c>
+      <c r="C58" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" t="s">
+        <v>103</v>
+      </c>
+      <c r="F58" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>103</v>
+      </c>
+      <c r="C59" t="s">
+        <v>102</v>
+      </c>
+      <c r="D59" t="s">
+        <v>106</v>
+      </c>
+      <c r="F59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>104</v>
+      </c>
+      <c r="C60" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>107</v>
+      </c>
+      <c r="C61" t="s">
+        <v>109</v>
+      </c>
+      <c r="D61" t="s">
+        <v>106</v>
+      </c>
+      <c r="F61" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>108</v>
+      </c>
+      <c r="C62" t="s">
+        <v>110</v>
+      </c>
+      <c r="D62" t="s">
+        <v>111</v>
+      </c>
+      <c r="F62" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>111</v>
+      </c>
+      <c r="C63" t="s">
+        <v>96</v>
+      </c>
+      <c r="D63" t="s">
+        <v>97</v>
+      </c>
+      <c r="F63" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>112</v>
+      </c>
+      <c r="C64" t="s">
+        <v>113</v>
+      </c>
+      <c r="D64" t="s">
+        <v>108</v>
+      </c>
+      <c r="F64" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>113</v>
+      </c>
+      <c r="C65" t="s">
+        <v>115</v>
+      </c>
+      <c r="D65" t="s">
+        <v>108</v>
+      </c>
+      <c r="F65" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>114</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D66" t="s">
+        <v>100</v>
+      </c>
+      <c r="F66" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F74" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75">
         <v>1290</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C75" t="s">
         <v>10</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D75" t="s">
         <v>12</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G75" s="3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F78" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F79" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{7EFC0B5E-D1D3-6743-B22B-C78E928786AB}"/>
-    <hyperlink ref="G47" r:id="rId2" xr:uid="{1C5B19B3-BCF2-FD46-9AE1-1F3B434170AD}"/>
+    <hyperlink ref="G75" r:id="rId2" xr:uid="{1C5B19B3-BCF2-FD46-9AE1-1F3B434170AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added few more good to solve problems in future.
</commit_message>
<xml_diff>
--- a/RevisionSheet.xlsx
+++ b/RevisionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milind.gokhale/git/jsdev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E3600D-0BE4-174B-BB99-319DF6977E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62BBD87-FF8D-5543-B35C-FEC9B1FC3E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t>Set Matrix Zeroes</t>
   </si>
   <si>
-    <t>Really good way of reducing space complexity.</t>
-  </si>
-  <si>
     <t>Search a 2D Matrix</t>
   </si>
   <si>
@@ -438,6 +435,12 @@
   </si>
   <si>
     <t>HashMap | Linear</t>
+  </si>
+  <si>
+    <t>Really good way of reducing space complexity.
+hint use the first index of row and column as the flagger to check whether we need to update this row and column to 0. Then iterate over the first row and first column and check and update respective rows and columns to 0.
+So whenever you encounter a cell with value 0, call updateRowCol function to update that cells i row and j column to $ for all cells which are Non-zero.
+Then run a similar double for loop to basically turn all $s into 0s.</t>
   </si>
 </sst>
 </file>
@@ -530,7 +533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -554,6 +557,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -864,7 +870,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -918,10 +924,10 @@
         <v>6</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
@@ -945,10 +951,10 @@
         <v>10</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -970,7 +976,7 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -988,16 +994,16 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1620,7 +1626,7 @@
     </row>
     <row r="47" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B47" s="3">
         <v>73</v>
@@ -1632,8 +1638,8 @@
         <v>41</v>
       </c>
       <c r="E47" s="2"/>
-      <c r="F47" s="2" t="s">
-        <v>63</v>
+      <c r="F47" s="13" t="s">
+        <v>136</v>
       </c>
       <c r="G47" s="2"/>
     </row>
@@ -1645,14 +1651,14 @@
         <v>74</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G48" s="2"/>
     </row>
@@ -1664,14 +1670,14 @@
         <v>75</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G49" s="2"/>
     </row>
@@ -1683,14 +1689,14 @@
         <v>80</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G50" s="2"/>
     </row>
@@ -1702,14 +1708,14 @@
         <v>82</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G51" s="2"/>
     </row>
@@ -1721,14 +1727,14 @@
         <v>83</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G52" s="2"/>
     </row>
@@ -1740,14 +1746,14 @@
         <v>86</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G53" s="2"/>
     </row>
@@ -1759,14 +1765,14 @@
         <v>88</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G54" s="2"/>
     </row>
@@ -1778,14 +1784,14 @@
         <v>94</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G55" s="2"/>
     </row>
@@ -1797,14 +1803,14 @@
         <v>100</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G56" s="2"/>
     </row>
@@ -1816,14 +1822,14 @@
         <v>101</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G57" s="2"/>
     </row>
@@ -1835,14 +1841,14 @@
         <v>102</v>
       </c>
       <c r="C58" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G58" s="2"/>
     </row>
@@ -1854,14 +1860,14 @@
         <v>103</v>
       </c>
       <c r="C59" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G59" s="2"/>
     </row>
@@ -1873,10 +1879,10 @@
         <v>104</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -1890,14 +1896,14 @@
         <v>107</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G61" s="2"/>
     </row>
@@ -1909,14 +1915,14 @@
         <v>108</v>
       </c>
       <c r="C62" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G62" s="2"/>
     </row>
@@ -1928,14 +1934,14 @@
         <v>111</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G63" s="2"/>
     </row>
@@ -1947,14 +1953,14 @@
         <v>112</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G64" s="2"/>
     </row>
@@ -1966,14 +1972,14 @@
         <v>113</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G65" s="2"/>
     </row>
@@ -1985,14 +1991,14 @@
         <v>114</v>
       </c>
       <c r="C66" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G66" s="2"/>
     </row>
@@ -2004,14 +2010,14 @@
         <v>117</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G67" s="2"/>
     </row>
@@ -2023,14 +2029,14 @@
         <v>121</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G68" s="2"/>
     </row>
@@ -2042,14 +2048,14 @@
         <v>122</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G69" s="2"/>
     </row>
@@ -2061,14 +2067,14 @@
         <v>124</v>
       </c>
       <c r="C70" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G70" s="2"/>
     </row>
@@ -2078,10 +2084,10 @@
         <v>383</v>
       </c>
       <c r="C71" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D71" s="10" t="s">
         <v>135</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>136</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -2112,7 +2118,7 @@
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G74" s="2"/>
     </row>
@@ -2124,17 +2130,17 @@
         <v>1290</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G75" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2162,7 +2168,7 @@
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G78" s="2"/>
     </row>
@@ -2173,7 +2179,7 @@
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G79" s="2"/>
     </row>

</xml_diff>